<commit_message>
Working more on the decoder model
</commit_message>
<xml_diff>
--- a/src/main/java/excel_decoder_files/smu_decoder_file.xlsx
+++ b/src/main/java/excel_decoder_files/smu_decoder_file.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\LaborDashboard\src\main\java\decoder_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\LaborDashboard\src\main\java\excel_decoder_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A28021A-7F3B-435B-94F3-15E376309E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D92094-64C3-42EF-9B9C-8E66C93804FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BF93DD93-9419-4F7C-BCB7-368AC606ADC2}"/>
+    <workbookView xWindow="11625" yWindow="0" windowWidth="17175" windowHeight="15600" activeTab="1" xr2:uid="{BF93DD93-9419-4F7C-BCB7-368AC606ADC2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Code Lists" sheetId="1" r:id="rId1"/>
-    <sheet name="Series ID Format" sheetId="3" r:id="rId2"/>
+    <sheet name="Series ID Format" sheetId="3" r:id="rId1"/>
+    <sheet name="Code Lists" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3248,11 +3248,118 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80EF634C-BF3C-4079-BECB-13603B55FE40}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="5" customFormat="1" ht="30">
+      <c r="A1" s="4" t="s">
+        <v>867</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>875</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>868</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>869</v>
+      </c>
+      <c r="B3" s="6">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="B4" s="6">
+        <v>4</v>
+      </c>
+      <c r="C4" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="B5" s="6">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>872</v>
+      </c>
+      <c r="B6" s="6">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="B7" s="6">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>874</v>
+      </c>
+      <c r="B8" s="6">
+        <v>19</v>
+      </c>
+      <c r="C8" s="6">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C84651-D6E8-4D91-AF9B-F62D7CCEFDA3}">
   <dimension ref="A1:P449"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9685,111 +9792,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80EF634C-BF3C-4079-BECB-13603B55FE40}">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="5" customFormat="1" ht="30">
-      <c r="A1" s="4" t="s">
-        <v>867</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>875</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>868</v>
-      </c>
-      <c r="B2" s="6">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
-        <v>869</v>
-      </c>
-      <c r="B3" s="6">
-        <v>3</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>870</v>
-      </c>
-      <c r="B4" s="6">
-        <v>4</v>
-      </c>
-      <c r="C4" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>871</v>
-      </c>
-      <c r="B5" s="6">
-        <v>6</v>
-      </c>
-      <c r="C5" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>872</v>
-      </c>
-      <c r="B6" s="6">
-        <v>11</v>
-      </c>
-      <c r="C6" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
-        <v>873</v>
-      </c>
-      <c r="B7" s="6">
-        <v>11</v>
-      </c>
-      <c r="C7" s="6">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
-        <v>874</v>
-      </c>
-      <c r="B8" s="6">
-        <v>19</v>
-      </c>
-      <c r="C8" s="6">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>